<commit_message>
Update files for reviews through #12
</commit_message>
<xml_diff>
--- a/DB files - Excel/tblStudyManagementTools.xlsx
+++ b/DB files - Excel/tblStudyManagementTools.xlsx
@@ -493,7 +493,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" rightToLeft="false">
       <selection activeCell="C5" sqref="C5"/>
@@ -989,6 +989,126 @@
         </is>
       </c>
     </row>
+    <row outlineLevel="0" r="25">
+      <c r="A25" s="4">
+        <v>24</v>
+      </c>
+      <c r="B25" s="4" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+      <c r="C25" s="5" t="inlineStr">
+        <is>
+          <t>Closures</t>
+        </is>
+      </c>
+      <c r="D25" s="6" t="inlineStr">
+        <is>
+          <t>Spatial Closures, of three types.  Marine protected areas, species risk based closures, and triggered closures based on effort</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="26">
+      <c r="A26" s="4">
+        <v>25</v>
+      </c>
+      <c r="B26" s="4" t="inlineStr">
+        <is>
+          <t>19</t>
+        </is>
+      </c>
+      <c r="C26" s="5" t="inlineStr">
+        <is>
+          <t>Catch Limit</t>
+        </is>
+      </c>
+      <c r="D26" s="6" t="inlineStr">
+        <is>
+          <t>four Landing regulations:  landing obligation, 5% discard limit, year-to-year quota transfer, both</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="27">
+      <c r="A27" s="4">
+        <v>26</v>
+      </c>
+      <c r="B27" s="4" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="C27" s="5" t="inlineStr">
+        <is>
+          <t>Effort Limit</t>
+        </is>
+      </c>
+      <c r="D27" s="6" t="inlineStr">
+        <is>
+          <t>None, the current method is used in all simulations</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="28">
+      <c r="A28" s="4">
+        <v>27</v>
+      </c>
+      <c r="B28" s="4" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="C28" s="5" t="inlineStr">
+        <is>
+          <t>Catch Limit</t>
+        </is>
+      </c>
+      <c r="D28" s="6" t="inlineStr">
+        <is>
+          <t>Status quo, 2x, Profit max, Broken stick control rule, Spatial broken stick control rule</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="29">
+      <c r="A29" s="4">
+        <v>28</v>
+      </c>
+      <c r="B29" s="4" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="C29" s="5" t="inlineStr">
+        <is>
+          <t>Closures</t>
+        </is>
+      </c>
+      <c r="D29" s="6" t="inlineStr">
+        <is>
+          <t>Spatial closures.  Closure trigger by zone or species with 20% or 30% triggers</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="30">
+      <c r="A30" s="4">
+        <v>29</v>
+      </c>
+      <c r="B30" s="4" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="C30" s="5" t="inlineStr">
+        <is>
+          <t>Catch Limit</t>
+        </is>
+      </c>
+      <c r="D30" s="6" t="inlineStr">
+        <is>
+          <t>8 approaches to setting P* buffer relative to F(lim).</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update excel files with new reviews
</commit_message>
<xml_diff>
--- a/DB files - Excel/tblStudyManagementTools.xlsx
+++ b/DB files - Excel/tblStudyManagementTools.xlsx
@@ -493,7 +493,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D43"/>
+  <dimension ref="A1:D75"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" rightToLeft="false">
       <selection activeCell="C5" sqref="C5"/>
@@ -1369,6 +1369,646 @@
         </is>
       </c>
     </row>
+    <row outlineLevel="0" r="44">
+      <c r="A44" s="4">
+        <v>44</v>
+      </c>
+      <c r="B44" s="4" t="inlineStr">
+        <is>
+          <t>41</t>
+        </is>
+      </c>
+      <c r="C44" s="5" t="inlineStr">
+        <is>
+          <t>Access Control</t>
+        </is>
+      </c>
+      <c r="D44" s="6" t="inlineStr">
+        <is>
+          <t>Constant across alternatives</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="45">
+      <c r="A45" s="4">
+        <v>45</v>
+      </c>
+      <c r="B45" s="4" t="inlineStr">
+        <is>
+          <t>41</t>
+        </is>
+      </c>
+      <c r="C45" s="5" t="inlineStr">
+        <is>
+          <t>Closures</t>
+        </is>
+      </c>
+      <c r="D45" s="6" t="inlineStr">
+        <is>
+          <t>4 temporal closure alternatives.  Base case, add May closure, add October closure, closure rule - if sample below threshold catch close</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="46">
+      <c r="A46" s="4">
+        <v>46</v>
+      </c>
+      <c r="B46" s="4" t="inlineStr">
+        <is>
+          <t>42</t>
+        </is>
+      </c>
+      <c r="C46" s="5" t="inlineStr">
+        <is>
+          <t>Catch Limit</t>
+        </is>
+      </c>
+      <c r="D46" s="6" t="inlineStr">
+        <is>
+          <t>Two HCRs, based on a static or a dynamic B(0) used as a BRP.</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="47">
+      <c r="A47" s="4">
+        <v>47</v>
+      </c>
+      <c r="B47" s="4" t="inlineStr">
+        <is>
+          <t>43</t>
+        </is>
+      </c>
+      <c r="C47" s="5" t="inlineStr">
+        <is>
+          <t>Catch Limit</t>
+        </is>
+      </c>
+      <c r="D47" s="6" t="inlineStr">
+        <is>
+          <t>Two HCRs, one with a constant F, and one with a variable F based on BRPs</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="48">
+      <c r="A48" s="4">
+        <v>48</v>
+      </c>
+      <c r="B48" s="4" t="inlineStr">
+        <is>
+          <t>43</t>
+        </is>
+      </c>
+      <c r="C48" s="5" t="inlineStr">
+        <is>
+          <t>Catch Limit</t>
+        </is>
+      </c>
+      <c r="D48" s="6" t="inlineStr">
+        <is>
+          <t>Two additional HCRs, which correspond to the first two, but are adjusted based on environmental conditions.</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="49">
+      <c r="A49" s="4">
+        <v>49</v>
+      </c>
+      <c r="B49" s="4" t="inlineStr">
+        <is>
+          <t>44</t>
+        </is>
+      </c>
+      <c r="C49" s="5" t="inlineStr">
+        <is>
+          <t>Catch Limit</t>
+        </is>
+      </c>
+      <c r="D49" s="6" t="inlineStr">
+        <is>
+          <t>4 management procedures covering different approaches to developing a rebuilding plan based on the acceptable recovery probability or inclusion of climate effects in the plan.</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="50">
+      <c r="A50" s="4">
+        <v>50</v>
+      </c>
+      <c r="B50" s="4" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+      <c r="C50" s="5" t="inlineStr">
+        <is>
+          <t>Catch Limit</t>
+        </is>
+      </c>
+      <c r="D50" s="6" t="inlineStr">
+        <is>
+          <t>This is a TAC based fishery.  The TACs weren't the focus, but would be altered by reference point changes.</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="51">
+      <c r="A51" s="4">
+        <v>51</v>
+      </c>
+      <c r="B51" s="4" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+      <c r="C51" s="5" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+      <c r="D51" s="6" t="inlineStr">
+        <is>
+          <t>Two reference point options, one that shifts to account for climate change, and one that does not.</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="52">
+      <c r="A52" s="4">
+        <v>52</v>
+      </c>
+      <c r="B52" s="4" t="inlineStr">
+        <is>
+          <t>46</t>
+        </is>
+      </c>
+      <c r="C52" s="5" t="inlineStr">
+        <is>
+          <t>Catch Limit</t>
+        </is>
+      </c>
+      <c r="D52" s="6" t="inlineStr">
+        <is>
+          <t>TAC implemented or not</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="53">
+      <c r="A53" s="4">
+        <v>53</v>
+      </c>
+      <c r="B53" s="4" t="inlineStr">
+        <is>
+          <t>46</t>
+        </is>
+      </c>
+      <c r="C53" s="5" t="inlineStr">
+        <is>
+          <t>Size Limit</t>
+        </is>
+      </c>
+      <c r="D53" s="6" t="inlineStr">
+        <is>
+          <t>Size limit implemented or not</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="54">
+      <c r="A54" s="4">
+        <v>54</v>
+      </c>
+      <c r="B54" s="4" t="inlineStr">
+        <is>
+          <t>46</t>
+        </is>
+      </c>
+      <c r="C54" s="5" t="inlineStr">
+        <is>
+          <t>Closures</t>
+        </is>
+      </c>
+      <c r="D54" s="6" t="inlineStr">
+        <is>
+          <t>marine protected areas implemented or not</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="55">
+      <c r="A55" s="4">
+        <v>55</v>
+      </c>
+      <c r="B55" s="4" t="inlineStr">
+        <is>
+          <t>46</t>
+        </is>
+      </c>
+      <c r="C55" s="5" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+      <c r="D55" s="6" t="inlineStr">
+        <is>
+          <t>Pollution reduction implemented or not</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="56">
+      <c r="A56" s="4">
+        <v>56</v>
+      </c>
+      <c r="B56" s="4" t="inlineStr">
+        <is>
+          <t>47</t>
+        </is>
+      </c>
+      <c r="C56" s="5" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+      <c r="D56" s="6" t="inlineStr">
+        <is>
+          <t>Note, not applicable to fishery management.  There are three approaches to beach replenishment, fixed amount and interval, fixed amount, and fixed interval, as well as no action.</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="57">
+      <c r="A57" s="4">
+        <v>57</v>
+      </c>
+      <c r="B57" s="4" t="inlineStr">
+        <is>
+          <t>48</t>
+        </is>
+      </c>
+      <c r="C57" s="5" t="inlineStr">
+        <is>
+          <t>Closures</t>
+        </is>
+      </c>
+      <c r="D57" s="6" t="inlineStr">
+        <is>
+          <t>Not cleared provided.</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="58">
+      <c r="A58" s="4">
+        <v>58</v>
+      </c>
+      <c r="B58" s="4" t="inlineStr">
+        <is>
+          <t>31</t>
+        </is>
+      </c>
+      <c r="C58" s="5" t="inlineStr">
+        <is>
+          <t>Closures</t>
+        </is>
+      </c>
+      <c r="D58" s="6" t="inlineStr">
+        <is>
+          <t>Spatial closures: No closures, 3 closure durations, 2 closure location rules</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="59">
+      <c r="A59" s="4">
+        <v>59</v>
+      </c>
+      <c r="B59" s="4" t="inlineStr">
+        <is>
+          <t>31</t>
+        </is>
+      </c>
+      <c r="C59" s="5" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+      <c r="D59" s="6" t="inlineStr">
+        <is>
+          <t>Size based closure rules: 4 options</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="60">
+      <c r="A60" s="4">
+        <v>60</v>
+      </c>
+      <c r="B60" s="4" t="inlineStr">
+        <is>
+          <t>49</t>
+        </is>
+      </c>
+      <c r="C60" s="5" t="inlineStr">
+        <is>
+          <t>Closures</t>
+        </is>
+      </c>
+      <c r="D60" s="6" t="inlineStr">
+        <is>
+          <t>Spatial closures: No closures, 3 closure durations, 2 closure location rules</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="61">
+      <c r="A61" s="4">
+        <v>61</v>
+      </c>
+      <c r="B61" s="4" t="inlineStr">
+        <is>
+          <t>49</t>
+        </is>
+      </c>
+      <c r="C61" s="5" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+      <c r="D61" s="6" t="inlineStr">
+        <is>
+          <t>Size based closure rules: 4 options</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="62">
+      <c r="A62" s="4">
+        <v>62</v>
+      </c>
+      <c r="B62" s="4" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="C62" s="5" t="inlineStr">
+        <is>
+          <t>Catch Limit</t>
+        </is>
+      </c>
+      <c r="D62" s="6" t="inlineStr">
+        <is>
+          <t>6 alternative methods for adjusting the catch limit.</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="63">
+      <c r="A63" s="4">
+        <v>63</v>
+      </c>
+      <c r="B63" s="4" t="inlineStr">
+        <is>
+          <t>32</t>
+        </is>
+      </c>
+      <c r="C63" s="5" t="inlineStr">
+        <is>
+          <t>Access Control, Catch Limit</t>
+        </is>
+      </c>
+      <c r="D63" s="6" t="inlineStr">
+        <is>
+          <t>Quota system, accompanied by location and gear restrictions, combined into 4 strategy</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="64">
+      <c r="A64" s="4">
+        <v>64</v>
+      </c>
+      <c r="B64" s="4" t="inlineStr">
+        <is>
+          <t>33</t>
+        </is>
+      </c>
+      <c r="C64" s="5" t="inlineStr">
+        <is>
+          <t>Size Limit</t>
+        </is>
+      </c>
+      <c r="D64" s="6" t="inlineStr">
+        <is>
+          <t># of size limits utilized and areas to which they are applied</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="65">
+      <c r="A65" s="4">
+        <v>65</v>
+      </c>
+      <c r="B65" s="4" t="inlineStr">
+        <is>
+          <t>34</t>
+        </is>
+      </c>
+      <c r="C65" s="5" t="inlineStr">
+        <is>
+          <t>Catch Limit, Effort Limit</t>
+        </is>
+      </c>
+      <c r="D65" s="6" t="inlineStr">
+        <is>
+          <t>22 MPs available in the DLMtoolkit package in R, 11 output control MPs and 11 input control MPs</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="66">
+      <c r="A66" s="4">
+        <v>66</v>
+      </c>
+      <c r="B66" s="4" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+      <c r="C66" s="5" t="inlineStr">
+        <is>
+          <t>Catch Limit</t>
+        </is>
+      </c>
+      <c r="D66" s="6" t="inlineStr">
+        <is>
+          <t>TAC=ABC set based on ICES F based proceedures (with and without uncertainty) and a constant F</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="67">
+      <c r="A67" s="4">
+        <v>67</v>
+      </c>
+      <c r="B67" s="4" t="inlineStr">
+        <is>
+          <t>36</t>
+        </is>
+      </c>
+      <c r="C67" s="5" t="inlineStr">
+        <is>
+          <t>Catch Limit</t>
+        </is>
+      </c>
+      <c r="D67" s="6" t="inlineStr">
+        <is>
+          <t>4 HCRs.  2 based on BRPs and 2 proportional harvest rules, the difference in each category is whether there is an annual TAC change limit.</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="68">
+      <c r="A68" s="4">
+        <v>68</v>
+      </c>
+      <c r="B68" s="4" t="inlineStr">
+        <is>
+          <t>36</t>
+        </is>
+      </c>
+      <c r="C68" s="5" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+      <c r="D68" s="6" t="inlineStr">
+        <is>
+          <t>3 stock assessment methods.  XSA, Schaefer, Difference</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="69">
+      <c r="A69" s="4">
+        <v>69</v>
+      </c>
+      <c r="B69" s="4" t="inlineStr">
+        <is>
+          <t>37</t>
+        </is>
+      </c>
+      <c r="C69" s="5" t="inlineStr">
+        <is>
+          <t>Effort Limit</t>
+        </is>
+      </c>
+      <c r="D69" s="6" t="inlineStr">
+        <is>
+          <t>2 levels, Status quo and reduction from 9000 to 5000 boat days</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="70">
+      <c r="A70" s="4">
+        <v>70</v>
+      </c>
+      <c r="B70" s="4" t="inlineStr">
+        <is>
+          <t>37</t>
+        </is>
+      </c>
+      <c r="C70" s="5" t="inlineStr">
+        <is>
+          <t>Closures</t>
+        </is>
+      </c>
+      <c r="D70" s="6" t="inlineStr">
+        <is>
+          <t>4 options, status quo, reef buffer area closure, Masig area closure, moon cycle calendar closure</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="71">
+      <c r="A71" s="4">
+        <v>71</v>
+      </c>
+      <c r="B71" s="4" t="inlineStr">
+        <is>
+          <t>38</t>
+        </is>
+      </c>
+      <c r="C71" s="5" t="inlineStr">
+        <is>
+          <t>Catch Limit</t>
+        </is>
+      </c>
+      <c r="D71" s="6" t="inlineStr">
+        <is>
+          <t>No alternatives, a single Harvest quota accompanied by a season duration</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="72">
+      <c r="A72" s="4">
+        <v>72</v>
+      </c>
+      <c r="B72" s="4" t="inlineStr">
+        <is>
+          <t>39</t>
+        </is>
+      </c>
+      <c r="C72" s="5" t="inlineStr">
+        <is>
+          <t>Catch Limit</t>
+        </is>
+      </c>
+      <c r="D72" s="6" t="inlineStr">
+        <is>
+          <t>4 TACs; 750 t, 1000 t, 1250 t, and 1500 t; competitave TAC vs ITQ</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="73">
+      <c r="A73" s="4">
+        <v>73</v>
+      </c>
+      <c r="B73" s="4" t="inlineStr">
+        <is>
+          <t>39</t>
+        </is>
+      </c>
+      <c r="C73" s="5" t="inlineStr">
+        <is>
+          <t>Effort Limit</t>
+        </is>
+      </c>
+      <c r="D73" s="6" t="inlineStr">
+        <is>
+          <t>constant effort limit</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="74">
+      <c r="A74" s="4">
+        <v>74</v>
+      </c>
+      <c r="B74" s="4" t="inlineStr">
+        <is>
+          <t>39</t>
+        </is>
+      </c>
+      <c r="C74" s="5" t="inlineStr">
+        <is>
+          <t>Closures</t>
+        </is>
+      </c>
+      <c r="D74" s="6" t="inlineStr">
+        <is>
+          <t>four spatially explicit no-take extents: an extent consistent with that from the mid-1980s to mid-2004 (approximately 16% of coral trout habitat in the park); an extent implemented during rezoning in 2004 (32%); a hypothetical extent of 50% (Little et al. 2009a); and a hypothetical extent of 0%.</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="75">
+      <c r="A75" s="4">
+        <v>75</v>
+      </c>
+      <c r="B75" s="4" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="C75" s="5" t="inlineStr">
+        <is>
+          <t>Catch Limit</t>
+        </is>
+      </c>
+      <c r="D75" s="6" t="inlineStr">
+        <is>
+          <t>6 HCRs combining timeline and precaution:  a reactive decision interval with no additional ACL reduction, and five HCRs consisting of a fixed decision interval with precautionary ACL reductions of 0 (i.e., no reduction), 10, 20, 30, and 40%.</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Database data file updates
</commit_message>
<xml_diff>
--- a/DB files - Excel/tblStudyManagementTools.xlsx
+++ b/DB files - Excel/tblStudyManagementTools.xlsx
@@ -493,7 +493,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D75"/>
+  <dimension ref="A1:D71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" rightToLeft="false">
       <selection activeCell="C5" sqref="C5"/>
@@ -691,171 +691,171 @@
     </row>
     <row outlineLevel="0" r="10">
       <c r="A10" s="4">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B10" s="4" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>11</t>
         </is>
       </c>
       <c r="C10" s="5" t="inlineStr">
         <is>
-          <t>Catch Limit</t>
+          <t>Effort Limit</t>
         </is>
       </c>
       <c r="D10" s="6" t="inlineStr">
         <is>
-          <t>Combinations of monitoring method and analytical methods</t>
+          <t>Four effort levels. Low, Moderate, High, and Very High effort equivalent to 80t, 110t, 140t, and 170t harvests.</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="11">
       <c r="A11" s="4">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B11" s="4" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>11</t>
         </is>
       </c>
       <c r="C11" s="5" t="inlineStr">
         <is>
-          <t>Catch Limit</t>
+          <t>Closure</t>
         </is>
       </c>
       <c r="D11" s="6" t="inlineStr">
         <is>
-          <t>Set of models used to forecast annual management adjustment</t>
+          <t>Two seasonal closures. Seasonal closure for 2 months or no closure.</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="12">
       <c r="A12" s="4">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B12" s="4" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>11</t>
         </is>
       </c>
       <c r="C12" s="5" t="inlineStr">
         <is>
-          <t>Closures</t>
+          <t>Closure</t>
         </is>
       </c>
       <c r="D12" s="6" t="inlineStr">
         <is>
-          <t>text</t>
+          <t>Two spatial closures. Spatial closure of 10 nautical miles around island or no closure.</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="13">
       <c r="A13" s="4">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B13" s="4" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>11</t>
         </is>
       </c>
       <c r="C13" s="5" t="inlineStr">
         <is>
-          <t>Share Allocation</t>
+          <t>Size Limit</t>
         </is>
       </c>
       <c r="D13" s="6" t="inlineStr">
         <is>
-          <t/>
+          <t>Three minimum size limits. 35, 38, and 40 cm TL.</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="14">
       <c r="A14" s="4">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B14" s="4" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>12</t>
         </is>
       </c>
       <c r="C14" s="5" t="inlineStr">
         <is>
-          <t>Effort Limit</t>
+          <t>Catch Limit</t>
         </is>
       </c>
       <c r="D14" s="6" t="inlineStr">
         <is>
-          <t>Four effort levels. Low, Moderate, High, and Very High effort equivalent to 80t, 110t, 140t, and 170t harvests.</t>
+          <t>Levels of adjustement to the catch limit to account for uncertainty</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="15">
       <c r="A15" s="4">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B15" s="4" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>13</t>
         </is>
       </c>
       <c r="C15" s="5" t="inlineStr">
         <is>
-          <t>Closures</t>
+          <t>Closure</t>
         </is>
       </c>
       <c r="D15" s="6" t="inlineStr">
         <is>
-          <t>Two seasonal closures. Seasonal closure for 2 months or no closure.</t>
+          <t>Three levels of area closure. Reef perimeter closed to fishing. 16%, 32%, 50% closed.</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="16">
       <c r="A16" s="4">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B16" s="4" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>13</t>
         </is>
       </c>
       <c r="C16" s="5" t="inlineStr">
         <is>
-          <t>Closures</t>
+          <t>Effort Limit</t>
         </is>
       </c>
       <c r="D16" s="6" t="inlineStr">
         <is>
-          <t>Two spatial closures. Spatial closure of 10 nautical miles around island or no closure.</t>
+          <t>Three levels of annual fishing effort. 0.5, 1, and 1.5 times 1996 effort.</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="17">
       <c r="A17" s="4">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B17" s="4" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>14</t>
         </is>
       </c>
       <c r="C17" s="5" t="inlineStr">
         <is>
-          <t>Size Limit</t>
+          <t>Catch Limit</t>
         </is>
       </c>
       <c r="D17" s="6" t="inlineStr">
         <is>
-          <t>Three minimum size limits. 35, 38, and 40 cm TL.</t>
+          <t>Harvest Control Rule sets target F, fishery mortality level.  HCR implementation method not specified.</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="18">
       <c r="A18" s="4">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B18" s="4" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>15</t>
         </is>
       </c>
       <c r="C18" s="5" t="inlineStr">
@@ -865,77 +865,77 @@
       </c>
       <c r="D18" s="6" t="inlineStr">
         <is>
-          <t>Levels of adjustement to the catch limit to account for uncertainty</t>
+          <t>Potential Biological Removal levels set as limit reference points, e.g. catch levels</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="19">
       <c r="A19" s="4">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B19" s="4" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>16</t>
         </is>
       </c>
       <c r="C19" s="5" t="inlineStr">
         <is>
-          <t>Closures</t>
+          <t>Catch Limit</t>
         </is>
       </c>
       <c r="D19" s="6" t="inlineStr">
         <is>
-          <t>Three levels of area closure. Reef perimeter closed to fishing. 16%, 32%, 50% closed.</t>
+          <t>Two harvest control rules were evaluated in three uncertainty scenarios each.</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="20">
       <c r="A20" s="4">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B20" s="4" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>17</t>
         </is>
       </c>
       <c r="C20" s="5" t="inlineStr">
         <is>
-          <t>Effort Limit</t>
+          <t>Catch Limit</t>
         </is>
       </c>
       <c r="D20" s="6" t="inlineStr">
         <is>
-          <t>Three levels of annual fishing effort. 0.5, 1, and 1.5 times 1996 effort.</t>
+          <t>Harvest Control Rule with TAC adjusted based on stock assessment output, specified by zone or region (zone area &gt; region area)</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="21">
       <c r="A21" s="4">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B21" s="4" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>18</t>
         </is>
       </c>
       <c r="C21" s="5" t="inlineStr">
         <is>
-          <t>Catch Limit</t>
+          <t>Closure</t>
         </is>
       </c>
       <c r="D21" s="6" t="inlineStr">
         <is>
-          <t>Harvest Control Rule sets target F, fishery mortality level.  HCR implementation method not specified.</t>
+          <t>Spatial Closures, of three types.  Marine protected areas, species risk based closures, and triggered closures based on effort</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="22">
       <c r="A22" s="4">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B22" s="4" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>19</t>
         </is>
       </c>
       <c r="C22" s="5" t="inlineStr">
@@ -945,37 +945,37 @@
       </c>
       <c r="D22" s="6" t="inlineStr">
         <is>
-          <t>Potential Biological Removal levels set as limit reference points, e.g. catch levels</t>
+          <t>four Landing regulations:  landing obligation, 5% discard limit, year-to-year quota transfer, both</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="23">
       <c r="A23" s="4">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B23" s="4" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>20</t>
         </is>
       </c>
       <c r="C23" s="5" t="inlineStr">
         <is>
-          <t>Catch Limit</t>
+          <t>Effort Limit</t>
         </is>
       </c>
       <c r="D23" s="6" t="inlineStr">
         <is>
-          <t>Two harvest control rules were evaluated in three uncertainty scenarios each.</t>
+          <t>None, the current method is used in all simulations</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="24">
       <c r="A24" s="4">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B24" s="4" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>21</t>
         </is>
       </c>
       <c r="C24" s="5" t="inlineStr">
@@ -985,37 +985,37 @@
       </c>
       <c r="D24" s="6" t="inlineStr">
         <is>
-          <t>Harvest Control Rule with TAC adjusted based on stock assessment output, specified by zone or region (zone area &gt; region area)</t>
+          <t>Status quo, 2x, Profit max, Broken stick control rule, Spatial broken stick control rule</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="25">
       <c r="A25" s="4">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B25" s="4" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>21</t>
         </is>
       </c>
       <c r="C25" s="5" t="inlineStr">
         <is>
-          <t>Closures</t>
+          <t>Closure</t>
         </is>
       </c>
       <c r="D25" s="6" t="inlineStr">
         <is>
-          <t>Spatial Closures, of three types.  Marine protected areas, species risk based closures, and triggered closures based on effort</t>
+          <t>Spatial closures.  Closure trigger by zone or species with 20% or 30% triggers</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="26">
       <c r="A26" s="4">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B26" s="4" t="inlineStr">
         <is>
-          <t>19</t>
+          <t>22</t>
         </is>
       </c>
       <c r="C26" s="5" t="inlineStr">
@@ -1025,77 +1025,77 @@
       </c>
       <c r="D26" s="6" t="inlineStr">
         <is>
-          <t>four Landing regulations:  landing obligation, 5% discard limit, year-to-year quota transfer, both</t>
+          <t>8 approaches to setting P* buffer relative to F(lim).</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="27">
       <c r="A27" s="4">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B27" s="4" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>23</t>
         </is>
       </c>
       <c r="C27" s="5" t="inlineStr">
         <is>
-          <t>Effort Limit</t>
+          <t>Catch Limit</t>
         </is>
       </c>
       <c r="D27" s="6" t="inlineStr">
         <is>
-          <t>None, the current method is used in all simulations</t>
+          <t>5 harvest quotas options</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="28">
       <c r="A28" s="4">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B28" s="4" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>23</t>
         </is>
       </c>
       <c r="C28" s="5" t="inlineStr">
         <is>
-          <t>Catch Limit</t>
+          <t>Closure</t>
         </is>
       </c>
       <c r="D28" s="6" t="inlineStr">
         <is>
-          <t>Status quo, 2x, Profit max, Broken stick control rule, Spatial broken stick control rule</t>
+          <t>Seasonal and area closures exist, but were constant across alternatives</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="29">
       <c r="A29" s="4">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B29" s="4" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>24</t>
         </is>
       </c>
       <c r="C29" s="5" t="inlineStr">
         <is>
-          <t>Closures</t>
+          <t>Catch Limit</t>
         </is>
       </c>
       <c r="D29" s="6" t="inlineStr">
         <is>
-          <t>Spatial closures.  Closure trigger by zone or species with 20% or 30% triggers</t>
+          <t>Catch limits set by HCR derived from monitoring methodology alternatives</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="30">
       <c r="A30" s="4">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B30" s="4" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>25</t>
         </is>
       </c>
       <c r="C30" s="5" t="inlineStr">
@@ -1105,57 +1105,57 @@
       </c>
       <c r="D30" s="6" t="inlineStr">
         <is>
-          <t>8 approaches to setting P* buffer relative to F(lim).</t>
+          <t>10% reduction annually until recovery achieved or no change</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="31">
       <c r="A31" s="4">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B31" s="4" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>25</t>
         </is>
       </c>
       <c r="C31" s="5" t="inlineStr">
         <is>
-          <t>Catch Limit</t>
+          <t>Effort Limit</t>
         </is>
       </c>
       <c r="D31" s="6" t="inlineStr">
         <is>
-          <t>5 harvest quotas options</t>
+          <t>10% reduction annually until recovery achieved or no change</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="32">
       <c r="A32" s="4">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="B32" s="4" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>25</t>
         </is>
       </c>
       <c r="C32" s="5" t="inlineStr">
         <is>
-          <t>Closures</t>
+          <t>Closure</t>
         </is>
       </c>
       <c r="D32" s="6" t="inlineStr">
         <is>
-          <t>Seasonal and area closures exist, but were constant across alternatives</t>
+          <t>Area closures, open or closed evaulated</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="33">
       <c r="A33" s="4">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B33" s="4" t="inlineStr">
         <is>
-          <t>24</t>
+          <t>26</t>
         </is>
       </c>
       <c r="C33" s="5" t="inlineStr">
@@ -1165,77 +1165,77 @@
       </c>
       <c r="D33" s="6" t="inlineStr">
         <is>
-          <t>Catch limits set by HCR derived from monitoring methodology alternatives</t>
+          <t>Limits set by a set of 4 Stock Assessment methodologies.</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="34">
       <c r="A34" s="4">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B34" s="4" t="inlineStr">
         <is>
-          <t>25</t>
+          <t>27</t>
         </is>
       </c>
       <c r="C34" s="5" t="inlineStr">
         <is>
-          <t>Catch Limit</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="D34" s="6" t="inlineStr">
         <is>
-          <t>10% reduction annually until recovery achieved or no change</t>
+          <t>Lamprey trapping options: Traps located in 14 or 16 streams, baited or unbaited.</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="35">
       <c r="A35" s="4">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="B35" s="4" t="inlineStr">
         <is>
-          <t>25</t>
+          <t>27</t>
         </is>
       </c>
       <c r="C35" s="5" t="inlineStr">
         <is>
-          <t>Effort Limit</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="D35" s="6" t="inlineStr">
         <is>
-          <t>10% reduction annually until recovery achieved or no change</t>
+          <t>Lamprey baiting options: Used fixed bait amount or achieve a target in-water concentration.</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="36">
       <c r="A36" s="4">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B36" s="4" t="inlineStr">
         <is>
-          <t>25</t>
+          <t>28</t>
         </is>
       </c>
       <c r="C36" s="5" t="inlineStr">
         <is>
-          <t>Closures</t>
+          <t>Closure, Size Limit</t>
         </is>
       </c>
       <c r="D36" s="6" t="inlineStr">
         <is>
-          <t>Area closures, open or closed evaulated</t>
+          <t>Not evaluated by analysis, single alternative is a sex, size, and season regulation system</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="37">
       <c r="A37" s="4">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B37" s="4" t="inlineStr">
         <is>
-          <t>26</t>
+          <t>29</t>
         </is>
       </c>
       <c r="C37" s="5" t="inlineStr">
@@ -1245,177 +1245,177 @@
       </c>
       <c r="D37" s="6" t="inlineStr">
         <is>
-          <t>Limits set by a set of 4 Stock Assessment methodologies.</t>
+          <t>Two TACC decision rule alternatives.</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="38">
       <c r="A38" s="4">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="B38" s="4" t="inlineStr">
         <is>
-          <t>27</t>
+          <t>30</t>
         </is>
       </c>
       <c r="C38" s="5" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Effort Limit</t>
         </is>
       </c>
       <c r="D38" s="6" t="inlineStr">
         <is>
-          <t>Lamprey trapping options: Traps located in 14 or 16 streams, baited or unbaited.</t>
+          <t>3 F based control rules.  Constant F, Reduced F when SSB&lt;0.4B(0), Reduced F when SSB&lt;0.7B(0),</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="39">
       <c r="A39" s="4">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B39" s="4" t="inlineStr">
         <is>
-          <t>27</t>
+          <t>30</t>
         </is>
       </c>
       <c r="C39" s="5" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Effort Limit</t>
         </is>
       </c>
       <c r="D39" s="6" t="inlineStr">
         <is>
-          <t>Lamprey baiting options: Used fixed bait amount or achieve a target in-water concentration.</t>
+          <t>7 baseline F levels.  0.1, 0.3, 0.5, 0.7, 1.0, 1.5, 2.0</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="40">
       <c r="A40" s="4">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="B40" s="4" t="inlineStr">
         <is>
-          <t>28</t>
+          <t>41</t>
         </is>
       </c>
       <c r="C40" s="5" t="inlineStr">
         <is>
-          <t>Closures, Size Limit</t>
+          <t>Access Control</t>
         </is>
       </c>
       <c r="D40" s="6" t="inlineStr">
         <is>
-          <t>Not evaluated by analysis, single alternative is a sex, size, and season regulation system</t>
+          <t>Constant across alternatives</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="41">
       <c r="A41" s="4">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="B41" s="4" t="inlineStr">
         <is>
-          <t>29</t>
+          <t>41</t>
         </is>
       </c>
       <c r="C41" s="5" t="inlineStr">
         <is>
-          <t>Catch Limit</t>
+          <t>Closure</t>
         </is>
       </c>
       <c r="D41" s="6" t="inlineStr">
         <is>
-          <t>Two TACC decision rule alternatives.</t>
+          <t>4 temporal closure alternatives.  Base case, add May closure, add October closure, closure rule - if sample below threshold catch close</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="42">
       <c r="A42" s="4">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B42" s="4" t="inlineStr">
         <is>
-          <t>30</t>
+          <t>42</t>
         </is>
       </c>
       <c r="C42" s="5" t="inlineStr">
         <is>
-          <t>Effort Limit</t>
+          <t>Catch Limit</t>
         </is>
       </c>
       <c r="D42" s="6" t="inlineStr">
         <is>
-          <t>3 F based control rules.  Constant F, Reduced F when SSB&lt;0.4B(0), Reduced F when SSB&lt;0.7B(0),</t>
+          <t>Two HCRs, based on a static or a dynamic B(0) used as a BRP.</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="43">
       <c r="A43" s="4">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="B43" s="4" t="inlineStr">
         <is>
-          <t>30</t>
+          <t>43</t>
         </is>
       </c>
       <c r="C43" s="5" t="inlineStr">
         <is>
-          <t>Effort Limit</t>
+          <t>Catch Limit</t>
         </is>
       </c>
       <c r="D43" s="6" t="inlineStr">
         <is>
-          <t>7 baseline F levels.  0.1, 0.3, 0.5, 0.7, 1.0, 1.5, 2.0</t>
+          <t>Two HCRs, one with a constant F, and one with a variable F based on BRPs</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="44">
       <c r="A44" s="4">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="B44" s="4" t="inlineStr">
         <is>
-          <t>41</t>
+          <t>43</t>
         </is>
       </c>
       <c r="C44" s="5" t="inlineStr">
         <is>
-          <t>Access Control</t>
+          <t>Catch Limit</t>
         </is>
       </c>
       <c r="D44" s="6" t="inlineStr">
         <is>
-          <t>Constant across alternatives</t>
+          <t>Two additional HCRs, which correspond to the first two, but are adjusted based on environmental conditions.</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="45">
       <c r="A45" s="4">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="B45" s="4" t="inlineStr">
         <is>
-          <t>41</t>
+          <t>44</t>
         </is>
       </c>
       <c r="C45" s="5" t="inlineStr">
         <is>
-          <t>Closures</t>
+          <t>Catch Limit</t>
         </is>
       </c>
       <c r="D45" s="6" t="inlineStr">
         <is>
-          <t>4 temporal closure alternatives.  Base case, add May closure, add October closure, closure rule - if sample below threshold catch close</t>
+          <t>4 management procedures covering different approaches to developing a rebuilding plan based on the acceptable recovery probability or inclusion of climate effects in the plan.</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="46">
       <c r="A46" s="4">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="B46" s="4" t="inlineStr">
         <is>
-          <t>42</t>
+          <t>45</t>
         </is>
       </c>
       <c r="C46" s="5" t="inlineStr">
@@ -1425,37 +1425,37 @@
       </c>
       <c r="D46" s="6" t="inlineStr">
         <is>
-          <t>Two HCRs, based on a static or a dynamic B(0) used as a BRP.</t>
+          <t>This is a TAC based fishery.  The TACs weren't the focus, but would be altered by reference point changes.</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="47">
       <c r="A47" s="4">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="B47" s="4" t="inlineStr">
         <is>
-          <t>43</t>
+          <t>45</t>
         </is>
       </c>
       <c r="C47" s="5" t="inlineStr">
         <is>
-          <t>Catch Limit</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="D47" s="6" t="inlineStr">
         <is>
-          <t>Two HCRs, one with a constant F, and one with a variable F based on BRPs</t>
+          <t>Two reference point options, one that shifts to account for climate change, and one that does not.</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="48">
       <c r="A48" s="4">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="B48" s="4" t="inlineStr">
         <is>
-          <t>43</t>
+          <t>46</t>
         </is>
       </c>
       <c r="C48" s="5" t="inlineStr">
@@ -1465,57 +1465,57 @@
       </c>
       <c r="D48" s="6" t="inlineStr">
         <is>
-          <t>Two additional HCRs, which correspond to the first two, but are adjusted based on environmental conditions.</t>
+          <t>TAC implemented or not</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="49">
       <c r="A49" s="4">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="B49" s="4" t="inlineStr">
         <is>
-          <t>44</t>
+          <t>46</t>
         </is>
       </c>
       <c r="C49" s="5" t="inlineStr">
         <is>
-          <t>Catch Limit</t>
+          <t>Size Limit</t>
         </is>
       </c>
       <c r="D49" s="6" t="inlineStr">
         <is>
-          <t>4 management procedures covering different approaches to developing a rebuilding plan based on the acceptable recovery probability or inclusion of climate effects in the plan.</t>
+          <t>Size limit implemented or not</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="50">
       <c r="A50" s="4">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="B50" s="4" t="inlineStr">
         <is>
-          <t>45</t>
+          <t>46</t>
         </is>
       </c>
       <c r="C50" s="5" t="inlineStr">
         <is>
-          <t>Catch Limit</t>
+          <t>Closure</t>
         </is>
       </c>
       <c r="D50" s="6" t="inlineStr">
         <is>
-          <t>This is a TAC based fishery.  The TACs weren't the focus, but would be altered by reference point changes.</t>
+          <t>marine protected areas implemented or not</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="51">
       <c r="A51" s="4">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="B51" s="4" t="inlineStr">
         <is>
-          <t>45</t>
+          <t>46</t>
         </is>
       </c>
       <c r="C51" s="5" t="inlineStr">
@@ -1525,77 +1525,77 @@
       </c>
       <c r="D51" s="6" t="inlineStr">
         <is>
-          <t>Two reference point options, one that shifts to account for climate change, and one that does not.</t>
+          <t>Pollution reduction implemented or not</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="52">
       <c r="A52" s="4">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="B52" s="4" t="inlineStr">
         <is>
-          <t>46</t>
+          <t>47</t>
         </is>
       </c>
       <c r="C52" s="5" t="inlineStr">
         <is>
-          <t>Catch Limit</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="D52" s="6" t="inlineStr">
         <is>
-          <t>TAC implemented or not</t>
+          <t>Note, not applicable to fishery management.  There are three approaches to beach replenishment, fixed amount and interval, fixed amount, and fixed interval, as well as no action.</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="53">
       <c r="A53" s="4">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="B53" s="4" t="inlineStr">
         <is>
-          <t>46</t>
+          <t>48</t>
         </is>
       </c>
       <c r="C53" s="5" t="inlineStr">
         <is>
-          <t>Size Limit</t>
+          <t>Closure</t>
         </is>
       </c>
       <c r="D53" s="6" t="inlineStr">
         <is>
-          <t>Size limit implemented or not</t>
+          <t>Not cleared provided.</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="54">
       <c r="A54" s="4">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="B54" s="4" t="inlineStr">
         <is>
-          <t>46</t>
+          <t>31</t>
         </is>
       </c>
       <c r="C54" s="5" t="inlineStr">
         <is>
-          <t>Closures</t>
+          <t>Closure</t>
         </is>
       </c>
       <c r="D54" s="6" t="inlineStr">
         <is>
-          <t>marine protected areas implemented or not</t>
+          <t>Spatial closures: No closures, 3 closure durations, 2 closure location rules</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="55">
       <c r="A55" s="4">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B55" s="4" t="inlineStr">
         <is>
-          <t>46</t>
+          <t>31</t>
         </is>
       </c>
       <c r="C55" s="5" t="inlineStr">
@@ -1605,137 +1605,137 @@
       </c>
       <c r="D55" s="6" t="inlineStr">
         <is>
-          <t>Pollution reduction implemented or not</t>
+          <t>Size based closure rules: 4 options</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="56">
       <c r="A56" s="4">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B56" s="4" t="inlineStr">
         <is>
-          <t>47</t>
+          <t>49</t>
         </is>
       </c>
       <c r="C56" s="5" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Closure</t>
         </is>
       </c>
       <c r="D56" s="6" t="inlineStr">
         <is>
-          <t>Note, not applicable to fishery management.  There are three approaches to beach replenishment, fixed amount and interval, fixed amount, and fixed interval, as well as no action.</t>
+          <t>Spatial closures: No closures, 3 closure durations, 2 closure location rules</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="57">
       <c r="A57" s="4">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B57" s="4" t="inlineStr">
         <is>
-          <t>48</t>
+          <t>49</t>
         </is>
       </c>
       <c r="C57" s="5" t="inlineStr">
         <is>
-          <t>Closures</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="D57" s="6" t="inlineStr">
         <is>
-          <t>Not cleared provided.</t>
+          <t>Size based closure rules: 4 options</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="58">
       <c r="A58" s="4">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="B58" s="4" t="inlineStr">
         <is>
-          <t>31</t>
+          <t>50</t>
         </is>
       </c>
       <c r="C58" s="5" t="inlineStr">
         <is>
-          <t>Closures</t>
+          <t>Catch Limit</t>
         </is>
       </c>
       <c r="D58" s="6" t="inlineStr">
         <is>
-          <t>Spatial closures: No closures, 3 closure durations, 2 closure location rules</t>
+          <t>6 alternative methods for adjusting the catch limit.</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="59">
       <c r="A59" s="4">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B59" s="4" t="inlineStr">
         <is>
-          <t>31</t>
+          <t>32</t>
         </is>
       </c>
       <c r="C59" s="5" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Access Control, Catch Limit</t>
         </is>
       </c>
       <c r="D59" s="6" t="inlineStr">
         <is>
-          <t>Size based closure rules: 4 options</t>
+          <t>Quota system, accompanied by location and gear restrictions, combined into 4 strategy</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="60">
       <c r="A60" s="4">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B60" s="4" t="inlineStr">
         <is>
-          <t>49</t>
+          <t>33</t>
         </is>
       </c>
       <c r="C60" s="5" t="inlineStr">
         <is>
-          <t>Closures</t>
+          <t>Size Limit</t>
         </is>
       </c>
       <c r="D60" s="6" t="inlineStr">
         <is>
-          <t>Spatial closures: No closures, 3 closure durations, 2 closure location rules</t>
+          <t># of size limits utilized and areas to which they are applied</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="61">
       <c r="A61" s="4">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B61" s="4" t="inlineStr">
         <is>
-          <t>49</t>
+          <t>34</t>
         </is>
       </c>
       <c r="C61" s="5" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Catch Limit, Effort Limit</t>
         </is>
       </c>
       <c r="D61" s="6" t="inlineStr">
         <is>
-          <t>Size based closure rules: 4 options</t>
+          <t>22 MPs available in the DLMtoolkit package in R, 11 output control MPs and 11 input control MPs</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="62">
       <c r="A62" s="4">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="B62" s="4" t="inlineStr">
         <is>
-          <t>50</t>
+          <t>35</t>
         </is>
       </c>
       <c r="C62" s="5" t="inlineStr">
@@ -1745,97 +1745,97 @@
       </c>
       <c r="D62" s="6" t="inlineStr">
         <is>
-          <t>6 alternative methods for adjusting the catch limit.</t>
+          <t>TAC=ABC set based on ICES F based proceedures (with and without uncertainty) and a constant F</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="63">
       <c r="A63" s="4">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="B63" s="4" t="inlineStr">
         <is>
-          <t>32</t>
+          <t>36</t>
         </is>
       </c>
       <c r="C63" s="5" t="inlineStr">
         <is>
-          <t>Access Control, Catch Limit</t>
+          <t>Catch Limit</t>
         </is>
       </c>
       <c r="D63" s="6" t="inlineStr">
         <is>
-          <t>Quota system, accompanied by location and gear restrictions, combined into 4 strategy</t>
+          <t>4 HCRs.  2 based on BRPs and 2 proportional harvest rules, the difference in each category is whether there is an annual TAC change limit.</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="64">
       <c r="A64" s="4">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="B64" s="4" t="inlineStr">
         <is>
-          <t>33</t>
+          <t>36</t>
         </is>
       </c>
       <c r="C64" s="5" t="inlineStr">
         <is>
-          <t>Size Limit</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="D64" s="6" t="inlineStr">
         <is>
-          <t># of size limits utilized and areas to which they are applied</t>
+          <t>3 stock assessment methods.  XSA, Schaefer, Difference</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="65">
       <c r="A65" s="4">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="B65" s="4" t="inlineStr">
         <is>
-          <t>34</t>
+          <t>37</t>
         </is>
       </c>
       <c r="C65" s="5" t="inlineStr">
         <is>
-          <t>Catch Limit, Effort Limit</t>
+          <t>Effort Limit</t>
         </is>
       </c>
       <c r="D65" s="6" t="inlineStr">
         <is>
-          <t>22 MPs available in the DLMtoolkit package in R, 11 output control MPs and 11 input control MPs</t>
+          <t>2 levels, Status quo and reduction from 9000 to 5000 boat days</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="66">
       <c r="A66" s="4">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="B66" s="4" t="inlineStr">
         <is>
-          <t>35</t>
+          <t>37</t>
         </is>
       </c>
       <c r="C66" s="5" t="inlineStr">
         <is>
-          <t>Catch Limit</t>
+          <t>Closure</t>
         </is>
       </c>
       <c r="D66" s="6" t="inlineStr">
         <is>
-          <t>TAC=ABC set based on ICES F based proceedures (with and without uncertainty) and a constant F</t>
+          <t>4 options, status quo, reef buffer area closure, Masig area closure, moon cycle calendar closure</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="67">
       <c r="A67" s="4">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="B67" s="4" t="inlineStr">
         <is>
-          <t>36</t>
+          <t>38</t>
         </is>
       </c>
       <c r="C67" s="5" t="inlineStr">
@@ -1845,37 +1845,37 @@
       </c>
       <c r="D67" s="6" t="inlineStr">
         <is>
-          <t>4 HCRs.  2 based on BRPs and 2 proportional harvest rules, the difference in each category is whether there is an annual TAC change limit.</t>
+          <t>No alternatives, a single Harvest quota accompanied by a season duration</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="68">
       <c r="A68" s="4">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="B68" s="4" t="inlineStr">
         <is>
-          <t>36</t>
+          <t>39</t>
         </is>
       </c>
       <c r="C68" s="5" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Catch Limit</t>
         </is>
       </c>
       <c r="D68" s="6" t="inlineStr">
         <is>
-          <t>3 stock assessment methods.  XSA, Schaefer, Difference</t>
+          <t>4 TACs; 750 t, 1000 t, 1250 t, and 1500 t; competitave TAC vs ITQ</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="69">
       <c r="A69" s="4">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="B69" s="4" t="inlineStr">
         <is>
-          <t>37</t>
+          <t>39</t>
         </is>
       </c>
       <c r="C69" s="5" t="inlineStr">
@@ -1885,37 +1885,37 @@
       </c>
       <c r="D69" s="6" t="inlineStr">
         <is>
-          <t>2 levels, Status quo and reduction from 9000 to 5000 boat days</t>
+          <t>constant effort limit</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="70">
       <c r="A70" s="4">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="B70" s="4" t="inlineStr">
         <is>
-          <t>37</t>
+          <t>39</t>
         </is>
       </c>
       <c r="C70" s="5" t="inlineStr">
         <is>
-          <t>Closures</t>
+          <t>Closure</t>
         </is>
       </c>
       <c r="D70" s="6" t="inlineStr">
         <is>
-          <t>4 options, status quo, reef buffer area closure, Masig area closure, moon cycle calendar closure</t>
+          <t>four spatially explicit no-take extents: an extent consistent with that from the mid-1980s to mid-2004 (approximately 16% of coral trout habitat in the park); an extent implemented during rezoning in 2004 (32%); a hypothetical extent of 50% (Little et al. 2009a); and a hypothetical extent of 0%.</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="71">
       <c r="A71" s="4">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="B71" s="4" t="inlineStr">
         <is>
-          <t>38</t>
+          <t>40</t>
         </is>
       </c>
       <c r="C71" s="5" t="inlineStr">
@@ -1924,86 +1924,6 @@
         </is>
       </c>
       <c r="D71" s="6" t="inlineStr">
-        <is>
-          <t>No alternatives, a single Harvest quota accompanied by a season duration</t>
-        </is>
-      </c>
-    </row>
-    <row outlineLevel="0" r="72">
-      <c r="A72" s="4">
-        <v>72</v>
-      </c>
-      <c r="B72" s="4" t="inlineStr">
-        <is>
-          <t>39</t>
-        </is>
-      </c>
-      <c r="C72" s="5" t="inlineStr">
-        <is>
-          <t>Catch Limit</t>
-        </is>
-      </c>
-      <c r="D72" s="6" t="inlineStr">
-        <is>
-          <t>4 TACs; 750 t, 1000 t, 1250 t, and 1500 t; competitave TAC vs ITQ</t>
-        </is>
-      </c>
-    </row>
-    <row outlineLevel="0" r="73">
-      <c r="A73" s="4">
-        <v>73</v>
-      </c>
-      <c r="B73" s="4" t="inlineStr">
-        <is>
-          <t>39</t>
-        </is>
-      </c>
-      <c r="C73" s="5" t="inlineStr">
-        <is>
-          <t>Effort Limit</t>
-        </is>
-      </c>
-      <c r="D73" s="6" t="inlineStr">
-        <is>
-          <t>constant effort limit</t>
-        </is>
-      </c>
-    </row>
-    <row outlineLevel="0" r="74">
-      <c r="A74" s="4">
-        <v>74</v>
-      </c>
-      <c r="B74" s="4" t="inlineStr">
-        <is>
-          <t>39</t>
-        </is>
-      </c>
-      <c r="C74" s="5" t="inlineStr">
-        <is>
-          <t>Closures</t>
-        </is>
-      </c>
-      <c r="D74" s="6" t="inlineStr">
-        <is>
-          <t>four spatially explicit no-take extents: an extent consistent with that from the mid-1980s to mid-2004 (approximately 16% of coral trout habitat in the park); an extent implemented during rezoning in 2004 (32%); a hypothetical extent of 50% (Little et al. 2009a); and a hypothetical extent of 0%.</t>
-        </is>
-      </c>
-    </row>
-    <row outlineLevel="0" r="75">
-      <c r="A75" s="4">
-        <v>75</v>
-      </c>
-      <c r="B75" s="4" t="inlineStr">
-        <is>
-          <t>40</t>
-        </is>
-      </c>
-      <c r="C75" s="5" t="inlineStr">
-        <is>
-          <t>Catch Limit</t>
-        </is>
-      </c>
-      <c r="D75" s="6" t="inlineStr">
         <is>
           <t>6 HCRs combining timeline and precaution:  a reactive decision interval with no additional ACL reduction, and five HCRs consisting of a fixed decision interval with precautionary ACL reductions of 0 (i.e., no reduction), 10, 20, 30, and 40%.</t>
         </is>

</xml_diff>